<commit_message>
added init overhead measurements
</commit_message>
<xml_diff>
--- a/archived/henschel/zcatoggleTest/ZCACost.xlsx
+++ b/archived/henschel/zcatoggleTest/ZCACost.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="20610" windowHeight="11655" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="20610" windowHeight="11640" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Overview ZCA" sheetId="9" r:id="rId1"/>
@@ -17,15 +17,17 @@
     <sheet name="LoopActivatedNotify" sheetId="8" r:id="rId8"/>
     <sheet name="EmpFunc_Dynaprof_no_backoff" sheetId="11" r:id="rId9"/>
     <sheet name="Loop_Dynaprof_no_backoff" sheetId="12" r:id="rId10"/>
-    <sheet name="old_Serial" sheetId="1" r:id="rId11"/>
-    <sheet name="old_OpenMP Parallel" sheetId="2" r:id="rId12"/>
+    <sheet name="EmpFunc_fixed_backoff" sheetId="13" r:id="rId11"/>
+    <sheet name="DynaProf_Init_Overhead" sheetId="14" r:id="rId12"/>
+    <sheet name="old_Serial" sheetId="1" r:id="rId13"/>
+    <sheet name="old_OpenMP Parallel" sheetId="2" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="94">
   <si>
     <t>Machine</t>
   </si>
@@ -261,6 +263,57 @@
   <si>
     <t>Empty loop with DynaProf NO-BACKOFF</t>
   </si>
+  <si>
+    <t>23_ActivatedNotifyFunction.cpp</t>
+  </si>
+  <si>
+    <t>export DYN_STRATEGY="FIXED_BACKOFF"</t>
+  </si>
+  <si>
+    <t>Back-Off Value</t>
+  </si>
+  <si>
+    <t>31_StartProfilerOverhead.cp1, 31_StartProfilerOverhead.cp2 and run_31.sh</t>
+  </si>
+  <si>
+    <t>The source code has an increasing number of functions with __notify_intrinsics</t>
+  </si>
+  <si>
+    <t>Functions with _notify_intrinsics</t>
+  </si>
+  <si>
+    <t>Number of __notify_intrinsics</t>
+  </si>
+  <si>
+    <t>Cycles for start_profiler()</t>
+  </si>
+  <si>
+    <t>This test is only done in serial.</t>
+  </si>
+  <si>
+    <t>Run "run_31.sh" to put the source together and run one test.</t>
+  </si>
+  <si>
+    <t>This test measures the time it takes to activate all __notify_intrinsics using DynaProf, with an increasing number of functions.</t>
+  </si>
+  <si>
+    <t>This test measures the time it takes to call a function that contains 2 activated __notify_intrinsic from a for loop with an increase FIXED_BACKOFF value.</t>
+  </si>
+  <si>
+    <t>export DYN_SAMPLE_SIZE="&lt;BACK_OFF_VALUE&gt;"</t>
+  </si>
+  <si>
+    <t>This test was only done in serial.</t>
+  </si>
+  <si>
+    <t>Avg Runtime in micro sec</t>
+  </si>
+  <si>
+    <t>Avg Runtime in milli sec</t>
+  </si>
+  <si>
+    <t>Avg [cycles] per Function</t>
+  </si>
 </sst>
 </file>
 
@@ -329,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -351,14 +404,17 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1777,11 +1833,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="118413568"/>
-        <c:axId val="118419840"/>
+        <c:axId val="118341632"/>
+        <c:axId val="118343552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="118413568"/>
+        <c:axId val="118341632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1803,14 +1859,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118419840"/>
+        <c:crossAx val="118343552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1818,7 +1873,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118419840"/>
+        <c:axId val="118343552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1841,21 +1896,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118413568"/>
+        <c:crossAx val="118341632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1900,7 +1953,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2167,11 +2219,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="118498048"/>
-        <c:axId val="118499968"/>
+        <c:axId val="119942144"/>
+        <c:axId val="119944320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="118498048"/>
+        <c:axId val="119942144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,14 +2245,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118499968"/>
+        <c:crossAx val="119944320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2208,7 +2259,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118499968"/>
+        <c:axId val="119944320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2231,21 +2282,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118498048"/>
+        <c:crossAx val="119942144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2285,12 +2334,742 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>DynaProf</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Fixed Back-Off</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EmpFunc_fixed_backoff!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg [cycles]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>EmpFunc_fixed_backoff!$B$12:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="#,##0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EmpFunc_fixed_backoff!$B$18:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>12.041369057280001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.041388165120001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.050913423360001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.09175643136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.543819264</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.906960773119998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.773077463039996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>509.54306558975998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="118810496"/>
+        <c:axId val="120258560"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="118810496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Back-Off Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120258560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="120258560"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cycles per Function Call</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="118810496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>DynaProf Fixed Back-Off</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EmpFunc_fixed_backoff!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg [cycles]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>EmpFunc_fixed_backoff!$B$20:$L$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0" formatCode="#,##0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EmpFunc_fixed_backoff!$B$26:$L$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>12.041235302400001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61.091070136319999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>109.54574352384</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>159.98621829119998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>207.48842317824</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>255.20080475136001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>308.02022470655999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>353.07293826047999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>407.04607048703997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>450.32186956800007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>498.06584595455996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="120291328"/>
+        <c:axId val="120293248"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="120291328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Back-Off Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120293248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="120293248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cycles per Function Call</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120291328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>Overhead in Cycles per</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
+              <a:t> Function with 2 __notify_intrinsics using DynaProf</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>DynaProf_Init_Overhead!$C$12:$Q$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DynaProf_Init_Overhead!$C$21:$Q$21</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>8551677.1999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4024387.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1959171.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1064434.5249999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>524708.27500000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>269873.15000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>153286.03125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94344.009374999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62296.990624999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46875.760546874997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38466.182812500003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32141.880273437499</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30107.228222656249</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28910.848681640626</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29153.394970703124</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="120408320"/>
+        <c:axId val="120410496"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="120408320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Functions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120410496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="120410496"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cycles per Function</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120408320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Cycles per Function Call</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2570,11 +3349,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="118874112"/>
-        <c:axId val="118876032"/>
+        <c:axId val="120351744"/>
+        <c:axId val="120353920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="118874112"/>
+        <c:axId val="120351744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2596,13 +3375,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118876032"/>
+        <c:crossAx val="120353920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2610,7 +3388,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118876032"/>
+        <c:axId val="120353920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2633,21 +3411,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118874112"/>
+        <c:crossAx val="120351744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2735,6 +3511,108 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4114,7 +4992,7 @@
   <dimension ref="A1:AI31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4354,7 +5232,7 @@
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="3">
@@ -4415,7 +5293,7 @@
       <c r="AI13" s="3"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="3">
         <v>503.89413841919998</v>
       </c>
@@ -4850,6 +5728,1737 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="I8" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="11">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>1000</v>
+      </c>
+      <c r="F12">
+        <v>10000</v>
+      </c>
+      <c r="G12">
+        <v>100000</v>
+      </c>
+      <c r="H12">
+        <v>100000</v>
+      </c>
+      <c r="I12">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="10">
+        <v>12.042286233600001</v>
+      </c>
+      <c r="C13" s="10">
+        <v>12.041569689599999</v>
+      </c>
+      <c r="D13" s="10">
+        <v>12.047731968000001</v>
+      </c>
+      <c r="E13" s="10">
+        <v>12.095071641600001</v>
+      </c>
+      <c r="F13" s="10">
+        <v>12.576207052799999</v>
+      </c>
+      <c r="G13" s="10">
+        <v>16.934562048</v>
+      </c>
+      <c r="H13" s="10">
+        <v>60.6494784</v>
+      </c>
+      <c r="I13" s="10">
+        <v>518.42259348480002</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="10">
+        <v>12.041235302400001</v>
+      </c>
+      <c r="C14" s="10">
+        <v>12.0428594688</v>
+      </c>
+      <c r="D14" s="10">
+        <v>12.045868953599999</v>
+      </c>
+      <c r="E14" s="10">
+        <v>12.090867916800001</v>
+      </c>
+      <c r="F14" s="10">
+        <v>12.525905664</v>
+      </c>
+      <c r="G14" s="10">
+        <v>16.895629824</v>
+      </c>
+      <c r="H14" s="10">
+        <v>60.834155673600002</v>
+      </c>
+      <c r="I14" s="10">
+        <v>498.7238435328</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="10">
+        <v>12.041378611200001</v>
+      </c>
+      <c r="C15" s="10">
+        <v>12.0407098368</v>
+      </c>
+      <c r="D15" s="10">
+        <v>12.045773414399999</v>
+      </c>
+      <c r="E15" s="10">
+        <v>12.089960294400001</v>
+      </c>
+      <c r="F15" s="10">
+        <v>12.5346952704</v>
+      </c>
+      <c r="G15" s="10">
+        <v>16.9052315136</v>
+      </c>
+      <c r="H15" s="10">
+        <v>60.862721894400003</v>
+      </c>
+      <c r="I15" s="10">
+        <v>524.83494574079998</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="10">
+        <v>12.041235302400001</v>
+      </c>
+      <c r="C16" s="10">
+        <v>12.041235302400001</v>
+      </c>
+      <c r="D16" s="10">
+        <v>12.044722483199999</v>
+      </c>
+      <c r="E16" s="10">
+        <v>12.094402867199999</v>
+      </c>
+      <c r="F16" s="10">
+        <v>12.535889510400001</v>
+      </c>
+      <c r="G16" s="10">
+        <v>16.901075558399999</v>
+      </c>
+      <c r="H16" s="10">
+        <v>60.715066060799998</v>
+      </c>
+      <c r="I16" s="10">
+        <v>507.51173022720002</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="10">
+        <v>12.0407098368</v>
+      </c>
+      <c r="C17" s="10">
+        <v>12.040566527999999</v>
+      </c>
+      <c r="D17" s="10">
+        <v>12.0704702976</v>
+      </c>
+      <c r="E17" s="10">
+        <v>12.0884794368</v>
+      </c>
+      <c r="F17" s="10">
+        <v>12.5463988224</v>
+      </c>
+      <c r="G17" s="10">
+        <v>16.898304921600001</v>
+      </c>
+      <c r="H17" s="10">
+        <v>60.8039652864</v>
+      </c>
+      <c r="I17" s="10">
+        <v>498.22221496319997</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="3"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="10">
+        <f>AVERAGE(B13:B17)</f>
+        <v>12.041369057280001</v>
+      </c>
+      <c r="C18" s="10">
+        <f t="shared" ref="C18:I18" si="0">AVERAGE(C13:C17)</f>
+        <v>12.041388165120001</v>
+      </c>
+      <c r="D18" s="10">
+        <f t="shared" si="0"/>
+        <v>12.050913423360001</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" si="0"/>
+        <v>12.09175643136</v>
+      </c>
+      <c r="F18" s="10">
+        <f t="shared" si="0"/>
+        <v>12.543819264</v>
+      </c>
+      <c r="G18" s="10">
+        <f t="shared" si="0"/>
+        <v>16.906960773119998</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="0"/>
+        <v>60.773077463039996</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="0"/>
+        <v>509.54306558975998</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="11">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1000000</v>
+      </c>
+      <c r="D20">
+        <f>C20+1000000</f>
+        <v>2000000</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20:L20" si="1">D20+1000000</f>
+        <v>3000000</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>4000000</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>5000000</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>6000000</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>7000000</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>8000000</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>9000000</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="10">
+        <v>12.041569689599999</v>
+      </c>
+      <c r="C21" s="10">
+        <v>60.617424998399997</v>
+      </c>
+      <c r="D21" s="10">
+        <v>109.26331054080001</v>
+      </c>
+      <c r="E21" s="10">
+        <v>158.02226672640001</v>
+      </c>
+      <c r="F21" s="10">
+        <v>211.42012876800001</v>
+      </c>
+      <c r="G21" s="10">
+        <v>255.08866083839999</v>
+      </c>
+      <c r="H21" s="10">
+        <v>312.16320568319998</v>
+      </c>
+      <c r="I21" s="10">
+        <v>352.35969991680003</v>
+      </c>
+      <c r="J21">
+        <v>419.79184051200002</v>
+      </c>
+      <c r="K21">
+        <v>450.00224317440001</v>
+      </c>
+      <c r="L21">
+        <v>498.20573445119999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="10">
+        <v>12.0428116992</v>
+      </c>
+      <c r="C22" s="10">
+        <v>62.516792064000001</v>
+      </c>
+      <c r="D22" s="10">
+        <v>111.13993927680001</v>
+      </c>
+      <c r="E22" s="10">
+        <v>167.6110585344</v>
+      </c>
+      <c r="F22" s="10">
+        <v>206.56425338880001</v>
+      </c>
+      <c r="G22" s="10">
+        <v>254.85903237119999</v>
+      </c>
+      <c r="H22" s="10">
+        <v>303.74519900159999</v>
+      </c>
+      <c r="I22" s="10">
+        <v>351.89943982080001</v>
+      </c>
+      <c r="J22">
+        <v>407.26545715200001</v>
+      </c>
+      <c r="K22">
+        <v>449.55836805119998</v>
+      </c>
+      <c r="L22">
+        <v>498.16976394239998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="10">
+        <v>12.0409486848</v>
+      </c>
+      <c r="C23" s="10">
+        <v>60.939392102399999</v>
+      </c>
+      <c r="D23" s="10">
+        <v>108.9140192256</v>
+      </c>
+      <c r="E23" s="10">
+        <v>158.675802624</v>
+      </c>
+      <c r="F23" s="10">
+        <v>206.49427092479999</v>
+      </c>
+      <c r="G23" s="10">
+        <v>255.0904760832</v>
+      </c>
+      <c r="H23" s="10">
+        <v>316.65092075519999</v>
+      </c>
+      <c r="I23" s="10">
+        <v>352.62324480000001</v>
+      </c>
+      <c r="J23">
+        <v>401.94664657919998</v>
+      </c>
+      <c r="K23">
+        <v>449.55927567359998</v>
+      </c>
+      <c r="L23">
+        <v>498.18399928320002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="10">
+        <v>12.0398022144</v>
+      </c>
+      <c r="C24" s="10">
+        <v>60.778026393600001</v>
+      </c>
+      <c r="D24" s="10">
+        <v>109.14049489919999</v>
+      </c>
+      <c r="E24" s="10">
+        <v>157.87628282879999</v>
+      </c>
+      <c r="F24" s="10">
+        <v>206.54003420160001</v>
+      </c>
+      <c r="G24" s="10">
+        <v>254.87508295679999</v>
+      </c>
+      <c r="H24" s="10">
+        <v>303.81155097599998</v>
+      </c>
+      <c r="I24" s="10">
+        <v>352.38143508479999</v>
+      </c>
+      <c r="J24">
+        <v>405.58946073599998</v>
+      </c>
+      <c r="K24">
+        <v>452.143085568</v>
+      </c>
+      <c r="L24">
+        <v>497.54594073599998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="10">
+        <v>12.041044224</v>
+      </c>
+      <c r="C25" s="10">
+        <v>60.603715123199997</v>
+      </c>
+      <c r="D25" s="10">
+        <v>109.2709536768</v>
+      </c>
+      <c r="E25" s="10">
+        <v>157.7456807424</v>
+      </c>
+      <c r="F25" s="10">
+        <v>206.42342860799999</v>
+      </c>
+      <c r="G25" s="10">
+        <v>256.09077150719997</v>
+      </c>
+      <c r="H25" s="10">
+        <v>303.7302471168</v>
+      </c>
+      <c r="I25" s="10">
+        <v>356.10087168000001</v>
+      </c>
+      <c r="J25">
+        <v>400.63694745599997</v>
+      </c>
+      <c r="K25">
+        <v>450.34637537280003</v>
+      </c>
+      <c r="L25">
+        <v>498.22379136000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="10">
+        <f>AVERAGE(B21:B25)</f>
+        <v>12.041235302400001</v>
+      </c>
+      <c r="C26" s="10">
+        <f t="shared" ref="C26" si="2">AVERAGE(C21:C25)</f>
+        <v>61.091070136319999</v>
+      </c>
+      <c r="D26" s="10">
+        <f t="shared" ref="D26" si="3">AVERAGE(D21:D25)</f>
+        <v>109.54574352384</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" ref="E26" si="4">AVERAGE(E21:E25)</f>
+        <v>159.98621829119998</v>
+      </c>
+      <c r="F26" s="10">
+        <f t="shared" ref="F26" si="5">AVERAGE(F21:F25)</f>
+        <v>207.48842317824</v>
+      </c>
+      <c r="G26" s="10">
+        <f t="shared" ref="G26" si="6">AVERAGE(G21:G25)</f>
+        <v>255.20080475136001</v>
+      </c>
+      <c r="H26" s="10">
+        <f t="shared" ref="H26" si="7">AVERAGE(H21:H25)</f>
+        <v>308.02022470655999</v>
+      </c>
+      <c r="I26" s="10">
+        <f t="shared" ref="I26" si="8">AVERAGE(I21:I25)</f>
+        <v>353.07293826047999</v>
+      </c>
+      <c r="J26" s="10">
+        <f t="shared" ref="J26" si="9">AVERAGE(J21:J25)</f>
+        <v>407.04607048703997</v>
+      </c>
+      <c r="K26" s="10">
+        <f t="shared" ref="K26" si="10">AVERAGE(K21:K25)</f>
+        <v>450.32186956800007</v>
+      </c>
+      <c r="L26" s="10">
+        <f t="shared" ref="L26" si="11">AVERAGE(L21:L25)</f>
+        <v>498.06584595455996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="10"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="10"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A21:A22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="15" max="17" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="I8" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="11">
+        <v>0</v>
+      </c>
+      <c r="C12" s="19">
+        <v>1</v>
+      </c>
+      <c r="D12" s="19">
+        <v>2</v>
+      </c>
+      <c r="E12" s="19">
+        <v>4</v>
+      </c>
+      <c r="F12" s="19">
+        <v>8</v>
+      </c>
+      <c r="G12" s="19">
+        <v>16</v>
+      </c>
+      <c r="H12" s="19">
+        <v>32</v>
+      </c>
+      <c r="I12" s="19">
+        <v>64</v>
+      </c>
+      <c r="J12" s="19">
+        <v>128</v>
+      </c>
+      <c r="K12" s="19">
+        <v>256</v>
+      </c>
+      <c r="L12" s="19">
+        <v>512</v>
+      </c>
+      <c r="M12" s="19">
+        <v>1024</v>
+      </c>
+      <c r="N12" s="19">
+        <v>2048</v>
+      </c>
+      <c r="O12" s="19">
+        <v>4096</v>
+      </c>
+      <c r="P12" s="19">
+        <v>8192</v>
+      </c>
+      <c r="Q12" s="19">
+        <f>P13</f>
+        <v>16384</v>
+      </c>
+      <c r="R12" s="19"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="11">
+        <f>B12*2</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="19">
+        <f t="shared" ref="C13:D13" si="0">C12*2</f>
+        <v>2</v>
+      </c>
+      <c r="D13" s="19">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E13" s="19">
+        <f t="shared" ref="E13" si="1">E12*2</f>
+        <v>8</v>
+      </c>
+      <c r="F13" s="19">
+        <f t="shared" ref="F13" si="2">F12*2</f>
+        <v>16</v>
+      </c>
+      <c r="G13" s="19">
+        <f t="shared" ref="G13" si="3">G12*2</f>
+        <v>32</v>
+      </c>
+      <c r="H13" s="19">
+        <f t="shared" ref="H13" si="4">H12*2</f>
+        <v>64</v>
+      </c>
+      <c r="I13" s="19">
+        <f t="shared" ref="I13:Q13" si="5">I12*2</f>
+        <v>128</v>
+      </c>
+      <c r="J13" s="19">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+      <c r="K13" s="19">
+        <f t="shared" si="5"/>
+        <v>512</v>
+      </c>
+      <c r="L13" s="19">
+        <f t="shared" si="5"/>
+        <v>1024</v>
+      </c>
+      <c r="M13" s="19">
+        <f t="shared" si="5"/>
+        <v>2048</v>
+      </c>
+      <c r="N13" s="19">
+        <f t="shared" si="5"/>
+        <v>4096</v>
+      </c>
+      <c r="O13" s="19">
+        <f t="shared" si="5"/>
+        <v>8192</v>
+      </c>
+      <c r="P13" s="19">
+        <f t="shared" si="5"/>
+        <v>16384</v>
+      </c>
+      <c r="Q13" s="19">
+        <f t="shared" si="5"/>
+        <v>32768</v>
+      </c>
+      <c r="R13" s="19"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8160468</v>
+      </c>
+      <c r="C14" s="3">
+        <v>8653060</v>
+      </c>
+      <c r="D14" s="3">
+        <v>9568778</v>
+      </c>
+      <c r="E14" s="3">
+        <v>7807376</v>
+      </c>
+      <c r="F14" s="3">
+        <v>9246982</v>
+      </c>
+      <c r="G14" s="3">
+        <v>8980436</v>
+      </c>
+      <c r="H14" s="3">
+        <v>8275392</v>
+      </c>
+      <c r="I14" s="3">
+        <v>10075600</v>
+      </c>
+      <c r="J14" s="3">
+        <v>12410068</v>
+      </c>
+      <c r="K14" s="3">
+        <v>18245388</v>
+      </c>
+      <c r="L14" s="3">
+        <v>25344014</v>
+      </c>
+      <c r="M14" s="3">
+        <v>41597178</v>
+      </c>
+      <c r="N14" s="3">
+        <v>64885226</v>
+      </c>
+      <c r="O14" s="3">
+        <v>123904394</v>
+      </c>
+      <c r="P14" s="3">
+        <v>238588902</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>478629334</v>
+      </c>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="3">
+        <v>8185950</v>
+      </c>
+      <c r="C15" s="3">
+        <v>8520220</v>
+      </c>
+      <c r="D15" s="3">
+        <v>7573852</v>
+      </c>
+      <c r="E15" s="3">
+        <v>8340484</v>
+      </c>
+      <c r="F15" s="3">
+        <v>8516249</v>
+      </c>
+      <c r="G15" s="3">
+        <v>8332722</v>
+      </c>
+      <c r="H15" s="3">
+        <v>9199898</v>
+      </c>
+      <c r="I15" s="3">
+        <v>10056382</v>
+      </c>
+      <c r="J15" s="3">
+        <v>11764362</v>
+      </c>
+      <c r="K15" s="3">
+        <v>15245754</v>
+      </c>
+      <c r="L15" s="3">
+        <v>24363630</v>
+      </c>
+      <c r="M15" s="3">
+        <v>38298470</v>
+      </c>
+      <c r="N15" s="3">
+        <v>65122674</v>
+      </c>
+      <c r="O15" s="3">
+        <v>122268444</v>
+      </c>
+      <c r="P15" s="3">
+        <v>235434672</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>475354288</v>
+      </c>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3">
+        <v>8375510</v>
+      </c>
+      <c r="C16" s="3">
+        <v>8557578</v>
+      </c>
+      <c r="D16" s="3">
+        <v>7560244</v>
+      </c>
+      <c r="E16" s="3">
+        <v>7705778</v>
+      </c>
+      <c r="F16" s="3">
+        <v>8991308</v>
+      </c>
+      <c r="G16" s="3">
+        <v>8189608</v>
+      </c>
+      <c r="H16" s="3">
+        <v>8513922</v>
+      </c>
+      <c r="I16" s="3">
+        <v>10137076</v>
+      </c>
+      <c r="J16" s="3">
+        <v>11729308</v>
+      </c>
+      <c r="K16" s="3">
+        <v>14451168</v>
+      </c>
+      <c r="L16" s="3">
+        <v>23625939</v>
+      </c>
+      <c r="M16" s="3">
+        <v>40923692</v>
+      </c>
+      <c r="N16" s="3">
+        <v>67283898</v>
+      </c>
+      <c r="O16" s="3">
+        <v>125339660</v>
+      </c>
+      <c r="P16" s="3">
+        <v>235965154</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>477649124</v>
+      </c>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3">
+        <v>8447284</v>
+      </c>
+      <c r="C17" s="3">
+        <v>8513764</v>
+      </c>
+      <c r="D17" s="3">
+        <v>7659052</v>
+      </c>
+      <c r="E17" s="3">
+        <v>7457082</v>
+      </c>
+      <c r="F17" s="3">
+        <v>7882546</v>
+      </c>
+      <c r="G17" s="3">
+        <v>8684714</v>
+      </c>
+      <c r="H17" s="3">
+        <v>8375626</v>
+      </c>
+      <c r="I17" s="3">
+        <v>9154050</v>
+      </c>
+      <c r="J17" s="3">
+        <v>12125492</v>
+      </c>
+      <c r="K17" s="3">
+        <v>15325486</v>
+      </c>
+      <c r="L17" s="3">
+        <v>23452614</v>
+      </c>
+      <c r="M17" s="3">
+        <v>38319854</v>
+      </c>
+      <c r="N17" s="3">
+        <v>66607130</v>
+      </c>
+      <c r="O17" s="3">
+        <v>122252136</v>
+      </c>
+      <c r="P17" s="3">
+        <v>236994510</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>480067040</v>
+      </c>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="3"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="3">
+        <v>8176264</v>
+      </c>
+      <c r="C18" s="3">
+        <v>8513764</v>
+      </c>
+      <c r="D18" s="3">
+        <v>7881948</v>
+      </c>
+      <c r="E18" s="3">
+        <v>7872708</v>
+      </c>
+      <c r="F18" s="3">
+        <v>7940296</v>
+      </c>
+      <c r="G18" s="3">
+        <v>7789182</v>
+      </c>
+      <c r="H18" s="3">
+        <v>8814866</v>
+      </c>
+      <c r="I18" s="3">
+        <v>9628422</v>
+      </c>
+      <c r="J18" s="3">
+        <v>12350936</v>
+      </c>
+      <c r="K18" s="3">
+        <v>16472352</v>
+      </c>
+      <c r="L18" s="3">
+        <v>23215750</v>
+      </c>
+      <c r="M18" s="3">
+        <v>37807662</v>
+      </c>
+      <c r="N18" s="3">
+        <v>65233926</v>
+      </c>
+      <c r="O18" s="3">
+        <v>122831400</v>
+      </c>
+      <c r="P18" s="3">
+        <v>237205124</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>476546330</v>
+      </c>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3">
+        <f>AVERAGE(B14:B18)</f>
+        <v>8269095.2000000002</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" ref="C19:L19" si="6">AVERAGE(C14:C18)</f>
+        <v>8551677.1999999993</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="6"/>
+        <v>8048774.7999999998</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="6"/>
+        <v>7836685.5999999996</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="6"/>
+        <v>8515476.1999999993</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="6"/>
+        <v>8395332.4000000004</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="6"/>
+        <v>8635940.8000000007</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="6"/>
+        <v>9810306</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="6"/>
+        <v>12076033.199999999</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="6"/>
+        <v>15948029.6</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" si="6"/>
+        <v>24000389.399999999</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" ref="M19:N19" si="7">AVERAGE(M14:M18)</f>
+        <v>39389371.200000003</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" si="7"/>
+        <v>65826570.799999997</v>
+      </c>
+      <c r="O19" s="3">
+        <f t="shared" ref="O19:P19" si="8">AVERAGE(O14:O18)</f>
+        <v>123319206.8</v>
+      </c>
+      <c r="P19" s="3">
+        <f t="shared" si="8"/>
+        <v>236837672.40000001</v>
+      </c>
+      <c r="Q19" s="3">
+        <f t="shared" ref="Q19" si="9">AVERAGE(Q14:Q18)</f>
+        <v>477649223.19999999</v>
+      </c>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="3"/>
+      <c r="AG19" s="3"/>
+      <c r="AH19" s="3"/>
+      <c r="AI19" s="3"/>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="10">
+        <f>B19*0.5359056806/1000/1000</f>
+        <v>4.431455091102193</v>
+      </c>
+      <c r="C20" s="10">
+        <f t="shared" ref="C20:Q20" si="10">C19*0.5359056806/1000/1000</f>
+        <v>4.582892390137502</v>
+      </c>
+      <c r="D20" s="10">
+        <f t="shared" si="10"/>
+        <v>4.3133841371901287</v>
+      </c>
+      <c r="E20" s="10">
+        <f t="shared" si="10"/>
+        <v>4.1997243301162186</v>
+      </c>
+      <c r="F20" s="10">
+        <f t="shared" si="10"/>
+        <v>4.5634920685941003</v>
+      </c>
+      <c r="G20" s="10">
+        <f t="shared" si="10"/>
+        <v>4.4991063236852318</v>
+      </c>
+      <c r="H20" s="10">
+        <f t="shared" si="10"/>
+        <v>4.6280497320453087</v>
+      </c>
+      <c r="I20" s="10">
+        <f t="shared" si="10"/>
+        <v>5.2573987138242639</v>
+      </c>
+      <c r="J20" s="10">
+        <f t="shared" si="10"/>
+        <v>6.4716147909941952</v>
+      </c>
+      <c r="K20" s="10">
+        <f t="shared" si="10"/>
+        <v>8.5466396570169447</v>
+      </c>
+      <c r="L20" s="10">
+        <f t="shared" si="10"/>
+        <v>12.861945016072024</v>
+      </c>
+      <c r="M20" s="10">
+        <f t="shared" si="10"/>
+        <v>21.108987781342037</v>
+      </c>
+      <c r="N20" s="10">
+        <f t="shared" si="10"/>
+        <v>35.276833226138088</v>
+      </c>
+      <c r="O20" s="10">
+        <f t="shared" si="10"/>
+        <v>66.087463451206148</v>
+      </c>
+      <c r="P20" s="10">
+        <f t="shared" si="10"/>
+        <v>126.92265401924183</v>
+      </c>
+      <c r="Q20" s="10">
+        <f t="shared" si="10"/>
+        <v>255.97493204705731</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3">
+        <f>C19/C12</f>
+        <v>8551677.1999999993</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" ref="D21:Q21" si="11">D19/D12</f>
+        <v>4024387.4</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="11"/>
+        <v>1959171.4</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="11"/>
+        <v>1064434.5249999999</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="11"/>
+        <v>524708.27500000002</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" si="11"/>
+        <v>269873.15000000002</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="11"/>
+        <v>153286.03125</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" si="11"/>
+        <v>94344.009374999994</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="11"/>
+        <v>62296.990624999999</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" si="11"/>
+        <v>46875.760546874997</v>
+      </c>
+      <c r="M21" s="3">
+        <f t="shared" si="11"/>
+        <v>38466.182812500003</v>
+      </c>
+      <c r="N21" s="3">
+        <f t="shared" si="11"/>
+        <v>32141.880273437499</v>
+      </c>
+      <c r="O21" s="3">
+        <f t="shared" si="11"/>
+        <v>30107.228222656249</v>
+      </c>
+      <c r="P21" s="3">
+        <f t="shared" si="11"/>
+        <v>28910.848681640626</v>
+      </c>
+      <c r="Q21" s="3">
+        <f t="shared" si="11"/>
+        <v>29153.394970703124</v>
+      </c>
+      <c r="R21" s="3"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10">
+        <f>C21*0.5359056806/1000</f>
+        <v>4582.8923901375019</v>
+      </c>
+      <c r="D22" s="10">
+        <f t="shared" ref="D22:Q22" si="12">D21*0.5359056806/1000</f>
+        <v>2156.6920685950645</v>
+      </c>
+      <c r="E22" s="10">
+        <f t="shared" si="12"/>
+        <v>1049.9310825290547</v>
+      </c>
+      <c r="F22" s="10">
+        <f t="shared" si="12"/>
+        <v>570.43650857426258</v>
+      </c>
+      <c r="G22" s="10">
+        <f t="shared" si="12"/>
+        <v>281.19414523032697</v>
+      </c>
+      <c r="H22" s="10">
+        <f t="shared" si="12"/>
+        <v>144.6265541264159</v>
+      </c>
+      <c r="I22" s="10">
+        <f t="shared" si="12"/>
+        <v>82.146854903504121</v>
+      </c>
+      <c r="J22" s="10">
+        <f t="shared" si="12"/>
+        <v>50.559490554642153</v>
+      </c>
+      <c r="K22" s="10">
+        <f t="shared" si="12"/>
+        <v>33.385311160222443</v>
+      </c>
+      <c r="L22" s="10">
+        <f t="shared" si="12"/>
+        <v>25.120986359515673</v>
+      </c>
+      <c r="M22" s="10">
+        <f t="shared" si="12"/>
+        <v>20.614245880216835</v>
+      </c>
+      <c r="N22" s="10">
+        <f t="shared" si="12"/>
+        <v>17.225016223700237</v>
+      </c>
+      <c r="O22" s="10">
+        <f t="shared" si="12"/>
+        <v>16.134634631642125</v>
+      </c>
+      <c r="P22" s="10">
+        <f t="shared" si="12"/>
+        <v>15.493488039458231</v>
+      </c>
+      <c r="Q22" s="10">
+        <f t="shared" si="12"/>
+        <v>15.623469973575276</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="10"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="10"/>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4941,7 +7550,7 @@
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -4949,7 +7558,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="21"/>
       <c r="B11">
         <v>11.085843302400001</v>
       </c>
@@ -4997,7 +7606,7 @@
       <c r="A18" s="1"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="20" t="s">
         <v>20</v>
       </c>
       <c r="B19">
@@ -5005,13 +7614,13 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
+      <c r="A20" s="20"/>
       <c r="B20">
         <v>27.377283225599999</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="6">
         <v>27.4674244608</v>
       </c>
@@ -5041,7 +7650,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="4">
@@ -5053,7 +7662,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+      <c r="A28" s="21"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
@@ -5073,7 +7682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG36"/>
   <sheetViews>
@@ -5265,7 +7874,7 @@
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="10">
@@ -5366,7 +7975,7 @@
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="10">
         <v>8.8186503167999994</v>
       </c>
@@ -6216,7 +8825,7 @@
       <c r="R20" s="10"/>
     </row>
     <row r="21" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="20" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="10">
@@ -6317,7 +8926,7 @@
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="10">
         <v>27.461596569600001</v>
       </c>
@@ -6416,7 +9025,7 @@
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="10">
         <v>27.461548799999999</v>
       </c>
@@ -7217,7 +9826,7 @@
       <c r="AG31" s="4"/>
     </row>
     <row r="32" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="10">
@@ -7350,7 +9959,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
+      <c r="A33" s="21"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
@@ -7375,8 +9984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8270,12 +10879,12 @@
       <c r="AH8" s="10"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="18" t="s">
         <v>73</v>
       </c>
       <c r="F10" s="10"/>
@@ -8550,7 +11159,7 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="10">
@@ -8654,7 +11263,7 @@
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="10">
         <v>12.039611136</v>
       </c>
@@ -9501,7 +12110,7 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="10">
@@ -9605,7 +12214,7 @@
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="10">
         <v>11.035732992</v>
       </c>
@@ -10452,7 +13061,7 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="10">
@@ -10556,7 +13165,7 @@
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="10">
         <v>27.414447974400002</v>
       </c>
@@ -11401,7 +14010,7 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="10">
@@ -11505,7 +14114,7 @@
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="10">
         <v>7.0281979392</v>
       </c>
@@ -12352,7 +14961,7 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="10">
@@ -12456,7 +15065,7 @@
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="10">
         <v>5.3348133887999998</v>
       </c>
@@ -13303,7 +15912,7 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="10">
@@ -13407,7 +16016,7 @@
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="10">
         <v>22.0685520384</v>
       </c>
@@ -14254,7 +16863,7 @@
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="3">
@@ -14333,7 +16942,7 @@
       <c r="AI13" s="3"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="3">
         <v>502.24551398400001</v>
       </c>

</xml_diff>